<commit_message>
add DTCO prediction and interpolation
</commit_message>
<xml_diff>
--- a/submission/2f96a5f92418_TGS.xlsx
+++ b/submission/2f96a5f92418_TGS.xlsx
@@ -396,7 +396,7 @@
         <v>12787.5</v>
       </c>
       <c r="B2">
-        <v>83.18822479248047</v>
+        <v>98.40113830566406</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -404,7 +404,7 @@
         <v>12788</v>
       </c>
       <c r="B3">
-        <v>83.27852630615234</v>
+        <v>98.49143981933594</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -13308,7 +13308,7 @@
         <v>13594.5</v>
       </c>
       <c r="B1616">
-        <v>103.9404296875</v>
+        <v>108.2292938232422</v>
       </c>
     </row>
     <row r="1617" spans="1:2">
@@ -13316,7 +13316,7 @@
         <v>13595</v>
       </c>
       <c r="B1617">
-        <v>102.929573059082</v>
+        <v>110.658203125</v>
       </c>
     </row>
     <row r="1618" spans="1:2">
@@ -13324,7 +13324,7 @@
         <v>13595.5</v>
       </c>
       <c r="B1618">
-        <v>104.3421401977539</v>
+        <v>113.7021636962891</v>
       </c>
     </row>
     <row r="1619" spans="1:2">
@@ -13332,7 +13332,7 @@
         <v>13596</v>
       </c>
       <c r="B1619">
-        <v>105.2410125732422</v>
+        <v>114.0236968994141</v>
       </c>
     </row>
     <row r="1620" spans="1:2">
@@ -13340,7 +13340,7 @@
         <v>13596.5</v>
       </c>
       <c r="B1620">
-        <v>117.0858688354492</v>
+        <v>118.059928894043</v>
       </c>
     </row>
     <row r="1621" spans="1:2">
@@ -13348,7 +13348,7 @@
         <v>13597</v>
       </c>
       <c r="B1621">
-        <v>109.0417938232422</v>
+        <v>116.7209930419922</v>
       </c>
     </row>
     <row r="1622" spans="1:2">
@@ -13356,7 +13356,7 @@
         <v>13597.5</v>
       </c>
       <c r="B1622">
-        <v>98.75404357910156</v>
+        <v>116.0920181274414</v>
       </c>
     </row>
     <row r="1623" spans="1:2">
@@ -13364,7 +13364,7 @@
         <v>13598</v>
       </c>
       <c r="B1623">
-        <v>106.4770584106445</v>
+        <v>122.3681945800781</v>
       </c>
     </row>
     <row r="1624" spans="1:2">
@@ -13372,7 +13372,7 @@
         <v>13598.5</v>
       </c>
       <c r="B1624">
-        <v>116.6284637451172</v>
+        <v>124.4242248535156</v>
       </c>
     </row>
     <row r="1625" spans="1:2">
@@ -28100,7 +28100,7 @@
         <v>14519</v>
       </c>
       <c r="B3465">
-        <v>136.5582275390625</v>
+        <v>135.3904113769531</v>
       </c>
     </row>
     <row r="3466" spans="1:2">
@@ -28108,7 +28108,7 @@
         <v>14519.5</v>
       </c>
       <c r="B3466">
-        <v>130.8426666259766</v>
+        <v>129.5810394287109</v>
       </c>
     </row>
     <row r="3467" spans="1:2">
@@ -28116,7 +28116,7 @@
         <v>14520</v>
       </c>
       <c r="B3467">
-        <v>122.1054077148438</v>
+        <v>129.0816192626953</v>
       </c>
     </row>
     <row r="3468" spans="1:2">
@@ -28124,7 +28124,7 @@
         <v>14520.5</v>
       </c>
       <c r="B3468">
-        <v>120.3858032226562</v>
+        <v>130.6165161132812</v>
       </c>
     </row>
     <row r="3469" spans="1:2">
@@ -28132,7 +28132,7 @@
         <v>14521</v>
       </c>
       <c r="B3469">
-        <v>122.8457183837891</v>
+        <v>127.8489761352539</v>
       </c>
     </row>
     <row r="3470" spans="1:2">
@@ -28140,7 +28140,7 @@
         <v>14521.5</v>
       </c>
       <c r="B3470">
-        <v>125.779052734375</v>
+        <v>123.2327728271484</v>
       </c>
     </row>
     <row r="3471" spans="1:2">
@@ -28148,7 +28148,7 @@
         <v>14522</v>
       </c>
       <c r="B3471">
-        <v>124.9921035766602</v>
+        <v>122.4458236694336</v>
       </c>
     </row>
     <row r="3472" spans="1:2">
@@ -28156,7 +28156,7 @@
         <v>14522.5</v>
       </c>
       <c r="B3472">
-        <v>124.4330596923828</v>
+        <v>121.8867797851562</v>
       </c>
     </row>
     <row r="3473" spans="1:2">
@@ -28164,7 +28164,7 @@
         <v>14523</v>
       </c>
       <c r="B3473">
-        <v>119.8677444458008</v>
+        <v>124.8710250854492</v>
       </c>
     </row>
     <row r="3474" spans="1:2">
@@ -28172,7 +28172,7 @@
         <v>14523.5</v>
       </c>
       <c r="B3474">
-        <v>120.2568435668945</v>
+        <v>127.6625823974609</v>
       </c>
     </row>
     <row r="3475" spans="1:2">
@@ -28180,7 +28180,7 @@
         <v>14524</v>
       </c>
       <c r="B3475">
-        <v>122.1054077148438</v>
+        <v>129.5111236572266</v>
       </c>
     </row>
     <row r="3476" spans="1:2">
@@ -28188,7 +28188,7 @@
         <v>14524.5</v>
       </c>
       <c r="B3476">
-        <v>122.765510559082</v>
+        <v>125.8444519042969</v>
       </c>
     </row>
     <row r="3477" spans="1:2">
@@ -28196,7 +28196,7 @@
         <v>14525</v>
       </c>
       <c r="B3477">
-        <v>127.0779800415039</v>
+        <v>126.9381408691406</v>
       </c>
     </row>
     <row r="3478" spans="1:2">
@@ -28204,7 +28204,7 @@
         <v>14525.5</v>
       </c>
       <c r="B3478">
-        <v>127.5381011962891</v>
+        <v>127.3982467651367</v>
       </c>
     </row>
     <row r="3479" spans="1:2">
@@ -28212,7 +28212,7 @@
         <v>14526</v>
       </c>
       <c r="B3479">
-        <v>129.6874694824219</v>
+        <v>129.5301666259766</v>
       </c>
     </row>
     <row r="3480" spans="1:2">
@@ -28220,7 +28220,7 @@
         <v>14526.5</v>
       </c>
       <c r="B3480">
-        <v>128.8380432128906</v>
+        <v>128.6807250976562</v>
       </c>
     </row>
     <row r="3481" spans="1:2">
@@ -28228,7 +28228,7 @@
         <v>14527</v>
       </c>
       <c r="B3481">
-        <v>128.715087890625</v>
+        <v>128.5751647949219</v>
       </c>
     </row>
     <row r="3482" spans="1:2">
@@ -28236,7 +28236,7 @@
         <v>14527.5</v>
       </c>
       <c r="B3482">
-        <v>128.5280303955078</v>
+        <v>127.3254623413086</v>
       </c>
     </row>
     <row r="3483" spans="1:2">
@@ -28244,7 +28244,7 @@
         <v>14528</v>
       </c>
       <c r="B3483">
-        <v>129.150146484375</v>
+        <v>127.1202621459961</v>
       </c>
     </row>
     <row r="3484" spans="1:2">
@@ -28252,7 +28252,7 @@
         <v>14528.5</v>
       </c>
       <c r="B3484">
-        <v>120.6758880615234</v>
+        <v>128.504150390625</v>
       </c>
     </row>
     <row r="3485" spans="1:2">
@@ -28260,7 +28260,7 @@
         <v>14529</v>
       </c>
       <c r="B3485">
-        <v>120.8327178955078</v>
+        <v>128.6609802246094</v>
       </c>
     </row>
     <row r="3486" spans="1:2">
@@ -28268,7 +28268,7 @@
         <v>14529.5</v>
       </c>
       <c r="B3486">
-        <v>122.4821624755859</v>
+        <v>129.8878784179688</v>
       </c>
     </row>
     <row r="3487" spans="1:2">
@@ -28276,7 +28276,7 @@
         <v>14530</v>
       </c>
       <c r="B3487">
-        <v>119.9606857299805</v>
+        <v>128.3123931884766</v>
       </c>
     </row>
     <row r="3488" spans="1:2">
@@ -28284,7 +28284,7 @@
         <v>14530.5</v>
       </c>
       <c r="B3488">
-        <v>119.4821929931641</v>
+        <v>127.404411315918</v>
       </c>
     </row>
     <row r="3489" spans="1:2">
@@ -28292,7 +28292,7 @@
         <v>14531</v>
       </c>
       <c r="B3489">
-        <v>128.9316558837891</v>
+        <v>128.7917327880859</v>
       </c>
     </row>
     <row r="3490" spans="1:2">
@@ -28300,7 +28300,7 @@
         <v>14531.5</v>
       </c>
       <c r="B3490">
-        <v>127.4095001220703</v>
+        <v>128.6270599365234</v>
       </c>
     </row>
     <row r="3491" spans="1:2">
@@ -28308,7 +28308,7 @@
         <v>14532</v>
       </c>
       <c r="B3491">
-        <v>127.6766357421875</v>
+        <v>129.5841064453125</v>
       </c>
     </row>
     <row r="3492" spans="1:2">
@@ -28316,7 +28316,7 @@
         <v>14532.5</v>
       </c>
       <c r="B3492">
-        <v>132.3114166259766</v>
+        <v>136.6270904541016</v>
       </c>
     </row>
     <row r="3493" spans="1:2">
@@ -28324,7 +28324,7 @@
         <v>14533</v>
       </c>
       <c r="B3493">
-        <v>131.3612823486328</v>
+        <v>135.6769714355469</v>
       </c>
     </row>
     <row r="3494" spans="1:2">
@@ -28332,7 +28332,7 @@
         <v>14533.5</v>
       </c>
       <c r="B3494">
-        <v>130.5780029296875</v>
+        <v>134.8936767578125</v>
       </c>
     </row>
     <row r="3495" spans="1:2">
@@ -28340,7 +28340,7 @@
         <v>14534</v>
       </c>
       <c r="B3495">
-        <v>130.2642211914062</v>
+        <v>135.4399261474609</v>
       </c>
     </row>
     <row r="3496" spans="1:2">
@@ -28348,7 +28348,7 @@
         <v>14534.5</v>
       </c>
       <c r="B3496">
-        <v>130.2642211914062</v>
+        <v>135.1198577880859</v>
       </c>
     </row>
     <row r="3497" spans="1:2">
@@ -28356,7 +28356,7 @@
         <v>14535</v>
       </c>
       <c r="B3497">
-        <v>131.5678558349609</v>
+        <v>136.4235076904297</v>
       </c>
     </row>
     <row r="3498" spans="1:2">
@@ -28364,7 +28364,7 @@
         <v>14535.5</v>
       </c>
       <c r="B3498">
-        <v>131.5678558349609</v>
+        <v>136.4235076904297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>